<commit_message>
Addded more stuff from CASA website
</commit_message>
<xml_diff>
--- a/doco/caliad.xlsx
+++ b/doco/caliad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendantwhite/code/caliad/doco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E440452C-F91E-6B4E-BCDA-0FA183E005B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F119E925-644A-A049-B5EA-5ADF0D5F2A8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="500" windowWidth="26340" windowHeight="10280" activeTab="6" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
     <workbookView xWindow="120" yWindow="8640" windowWidth="28600" windowHeight="8220" activeTab="10" xr2:uid="{9B7FAC73-210A-1C4C-B0D1-A025AF15558B}"/>
   </bookViews>
   <sheets>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9441" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9447" uniqueCount="1147">
   <si>
     <t>Adelaide Hills</t>
   </si>
@@ -3961,6 +3961,12 @@
   </si>
   <si>
     <t>Max Time</t>
+  </si>
+  <si>
+    <t>Short Name</t>
+  </si>
+  <si>
+    <t>Full Name</t>
   </si>
 </sst>
 </file>
@@ -4524,9 +4530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD349239-A764-1A46-BD88-AF5CB97580BD}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
     <sheetView workbookViewId="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
@@ -4645,7 +4653,7 @@
         <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>1146</v>
       </c>
       <c r="E7" t="s">
         <v>157</v>
@@ -4682,6 +4690,9 @@
       <c r="B8" t="s">
         <v>1137</v>
       </c>
+      <c r="D8" t="s">
+        <v>1145</v>
+      </c>
       <c r="E8" t="s">
         <v>1138</v>
       </c>
@@ -4690,6 +4701,31 @@
       </c>
       <c r="N8" t="s">
         <v>1144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -29167,7 +29203,7 @@
         <v>127</v>
       </c>
       <c r="J386" s="9" t="str">
-        <f t="shared" ref="J386:J449" si="6">SUBSTITUTE(SUBSTITUTE(K386,I386&amp;" ",""),I386,"")</f>
+        <f t="shared" ref="J386:J435" si="6">SUBSTITUTE(SUBSTITUTE(K386,I386&amp;" ",""),I386,"")</f>
         <v>Junior</v>
       </c>
       <c r="K386" s="25" t="s">
@@ -31115,7 +31151,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD53"/>
     </sheetView>
@@ -45516,7 +45552,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>

</xml_diff>

<commit_message>
updates - making them green as I create the database tables
</commit_message>
<xml_diff>
--- a/doco/caliad.xlsx
+++ b/doco/caliad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendantwhite/code/caliad/doco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAB69EA-B026-394B-8BEC-AA10E74A13F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8541BE1F-0291-D445-BE9E-6FB9E3C31B56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="10000" windowHeight="12880" activeTab="8" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="12" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Programme (ORIGINAL)'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Programme1!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Programme3!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Regions!$A$1:$C$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Item Rotation'!$A$1:$G$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9584" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9636" uniqueCount="1179">
   <si>
     <t>Adelaide Hills</t>
   </si>
@@ -3936,9 +3937,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Month/s</t>
   </si>
   <si>
     <t>Rank</t>
@@ -4071,6 +4069,24 @@
   </si>
   <si>
     <t>Duos</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Competitive Tinies </t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Laravel</t>
   </si>
 </sst>
 </file>
@@ -4300,7 +4316,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4421,15 +4437,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4451,12 +4458,25 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4828,45 +4848,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD349239-A764-1A46-BD88-AF5CB97580BD}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="6" width="13.83203125" style="64"/>
+    <col min="9" max="10" width="13.83203125" style="64"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="62" t="s">
         <v>1121</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="62" t="s">
         <v>944</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="62" t="s">
         <v>1087</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="62" t="s">
         <v>1133</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="62" t="s">
         <v>1127</v>
       </c>
       <c r="G1" s="39" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H1" s="39" t="s">
         <v>1108</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="I1" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="J1" s="62" t="s">
         <v>1126</v>
-      </c>
-      <c r="J1" s="39" t="s">
-        <v>1131</v>
       </c>
       <c r="K1" s="39" t="s">
         <v>950</v>
@@ -4878,22 +4900,27 @@
         <v>1129</v>
       </c>
       <c r="N1" s="39" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="45" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="63"/>
+      <c r="F2" s="63" t="s">
         <v>1133</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="H2" s="45" t="s">
         <v>1127</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="I2" s="63" t="s">
         <v>1126</v>
       </c>
+      <c r="J2" s="63"/>
       <c r="K2" s="45" t="s">
         <v>1087</v>
       </c>
@@ -4903,11 +4930,22 @@
       <c r="M2" s="45" t="s">
         <v>950</v>
       </c>
+      <c r="N2" s="45" t="s">
+        <v>1121</v>
+      </c>
     </row>
     <row r="3" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G3" s="45" t="s">
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="H3" s="45" t="s">
         <v>1121</v>
       </c>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
       <c r="K3" s="45" t="s">
         <v>1121</v>
       </c>
@@ -4917,106 +4955,140 @@
       <c r="M3" s="45" t="s">
         <v>1128</v>
       </c>
+      <c r="N3" s="45" t="s">
+        <v>1126</v>
+      </c>
     </row>
     <row r="4" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G4" s="45" t="s">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="H4" s="45" t="s">
         <v>1130</v>
       </c>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
       <c r="K4" s="45" t="s">
         <v>1131</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="45" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="H5" s="45" t="s">
         <v>1132</v>
       </c>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
       <c r="K5" s="45" t="s">
         <v>1133</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="D7" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="64" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E7" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="64" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" t="s">
         <v>1136</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="H7" s="46" t="s">
         <v>1135</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="I7" s="65" t="s">
+        <v>1145</v>
+      </c>
+      <c r="J7" s="65" t="s">
+        <v>157</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1140</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1140</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="64" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B8" s="64" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D8" s="64" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>1175</v>
+      </c>
+      <c r="I8" s="64" t="s">
+        <v>1144</v>
+      </c>
+      <c r="J8" s="64" t="s">
         <v>1139</v>
       </c>
-      <c r="I7" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1137</v>
-      </c>
-      <c r="L7" t="s">
-        <v>1141</v>
-      </c>
-      <c r="M7" t="s">
-        <v>1141</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="N8" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1145</v>
-      </c>
-      <c r="E8" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D9" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="64" t="s">
+        <v>1176</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>1173</v>
+      </c>
+      <c r="J9" s="65" t="s">
         <v>1138</v>
       </c>
-      <c r="I8" t="s">
-        <v>1140</v>
-      </c>
-      <c r="N8" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+      <c r="D10" s="64" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+      <c r="D11" s="64" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
+      <c r="D12" s="64" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
+      <c r="D13" s="64" t="s">
         <v>162</v>
       </c>
     </row>
@@ -5160,13 +5232,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE05866-F710-F341-B238-1B26866DF8B8}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2:K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5174,15 +5246,15 @@
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="9" width="26" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>249</v>
       </c>
@@ -5193,10 +5265,10 @@
         <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>157</v>
+        <v>1145</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>184</v>
+        <v>1144</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>161</v>
@@ -5210,8 +5282,14 @@
       <c r="I1" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5237,8 +5315,29 @@
       <c r="H2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K2" t="str">
+        <f>_xlfn.CONCAT("                'region_id'  =&gt; "&amp;A2&amp;", 
+","                'full_name'  =&gt; '"&amp;D2&amp;"', 
+","                'short_name' =&gt; '"&amp;E2&amp;"', 
+","                'contact'    =&gt; '"&amp;F2&amp;"', 
+","                'email'      =&gt; '"&amp;G2&amp;"', 
+","                'location'   =&gt; '"&amp;H2&amp;"', 
+","                'website'    =&gt; '"&amp;I2&amp;"', 
+            ],")</f>
+        <v xml:space="preserve">                'region_id'  =&gt; 1, 
+                'full_name'  =&gt; 'Jayde Calisthenics Academy', 
+                'short_name' =&gt; 'Jayde', 
+                'contact'    =&gt; 'Felicity Vardon 0468 534 646', 
+                'email'      =&gt; 'jaydecali@gmail', 
+                'location'   =&gt; 'Aldgate Memorial Hall', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5264,8 +5363,29 @@
       <c r="H3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K43" si="0">_xlfn.CONCAT("                'region_id'  =&gt; "&amp;A3&amp;", 
+","                'full_name'  =&gt; '"&amp;D3&amp;"', 
+","                'short_name' =&gt; '"&amp;E3&amp;"', 
+","                'contact'    =&gt; '"&amp;F3&amp;"', 
+","                'email'      =&gt; '"&amp;G3&amp;"', 
+","                'location'   =&gt; '"&amp;H3&amp;"', 
+","                'website'    =&gt; '"&amp;I3&amp;"', 
+            ],")</f>
+        <v xml:space="preserve">                'region_id'  =&gt; 1, 
+                'full_name'  =&gt; 'Acacia (Littlehampton/ Mt Barker)', 
+                'short_name' =&gt; 'Acacia', 
+                'contact'    =&gt; 'Katie : 0411094070', 
+                'email'      =&gt; 'secretary@acacia.dance', 
+                'location'   =&gt; 'Anembo Park, Littlehampton', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5291,8 +5411,22 @@
       <c r="I4" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 1, 
+                'full_name'  =&gt; 'Innovation Calisthenics Club Incorporated', 
+                'short_name' =&gt; 'Innovation ', 
+                'contact'    =&gt; 'Principal Coach Kate Loveridge ph 0409 270 877', 
+                'email'      =&gt; 'innovationcalisthenics@hotmail.com', 
+                'location'   =&gt; '', 
+                'website'    =&gt; 'www.innovationcalisthenicsclub.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5318,8 +5452,22 @@
       <c r="H5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 1, 
+                'full_name'  =&gt; 'Murray Bridge Calisthenics Club', 
+                'short_name' =&gt; 'Murray Bridge ', 
+                'contact'    =&gt; 'Leanne : 0407976635', 
+                'email'      =&gt; 'murraybridgecalisthenicsclub@outlook.com', 
+                'location'   =&gt; 'Murray Bridge', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5342,8 +5490,22 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 1, 
+                'full_name'  =&gt; 'Onkaparinga', 
+                'short_name' =&gt; 'Onkaparinga', 
+                'contact'    =&gt; 'Debbie McKay 0404 079 240', 
+                'email'      =&gt; '', 
+                'location'   =&gt; 'Oakbank Soldiers Memorial Hall, Main Rd, Oakbank', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -5366,8 +5528,22 @@
       <c r="H7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 2, 
+                'full_name'  =&gt; 'Gawler', 
+                'short_name' =&gt; 'Gawler', 
+                'contact'    =&gt; '', 
+                'email'      =&gt; 'gawlercali@gmail.com', 
+                'location'   =&gt; 'Gawler Institute', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5393,8 +5569,22 @@
       <c r="I8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 3, 
+                'full_name'  =&gt; 'AVV Millennium Calisthenics and Dance Academy', 
+                'short_name' =&gt; 'AVV Millennium ', 
+                'contact'    =&gt; 'Karen Costanzo: 0438999367', 
+                'email'      =&gt; 'Karen.costanzo1@gmail.com', 
+                'location'   =&gt; '', 
+                'website'    =&gt; 'www.avvm.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -5423,8 +5613,22 @@
       <c r="I9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 3, 
+                'full_name'  =&gt; 'Burnside Calisthenics &amp; Dance Academy', 
+                'short_name' =&gt; 'Burnside ', 
+                'contact'    =&gt; 'Vicki on 0426 259 957', 
+                'email'      =&gt; 'secretary@burnsideacademy.com.au', 
+                'location'   =&gt; 'Unit 2, 20 Fullarton Road Norwood', 
+                'website'    =&gt; 'www.burnsideacademy.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5450,8 +5654,22 @@
       <c r="H10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 3, 
+                'full_name'  =&gt; 'Marden Calisthenics', 
+                'short_name' =&gt; 'Marden ', 
+                'contact'    =&gt; 'Nikki Ianunzio 0412 711 716', 
+                'email'      =&gt; 'nicktrick82@gmail.com', 
+                'location'   =&gt; 'St Josephs Hectorville', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -5477,8 +5695,22 @@
       <c r="H11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 3, 
+                'full_name'  =&gt; 'Waratah', 
+                'short_name' =&gt; 'Waratah', 
+                'contact'    =&gt; 'Lee-Ann Lewis 0466 637 343', 
+                'email'      =&gt; 'Waratahcalisthenics@gmail.com', 
+                'location'   =&gt; 'Athelstone', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -5507,8 +5739,22 @@
       <c r="I12" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 4, 
+                'full_name'  =&gt; 'Happy Valley', 
+                'short_name' =&gt; 'Happy Valley', 
+                'contact'    =&gt; 'Jessica Catford - 0401450864', 
+                'email'      =&gt; 'hvcalisthenics@hotmail.com', 
+                'location'   =&gt; 'Happy Valley Primary, Education Rd', 
+                'website'    =&gt; 'www.hvcalisthenics.com', 
+            ],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -5534,8 +5780,22 @@
       <c r="H13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 4, 
+                'full_name'  =&gt; 'Reynella-Braeview School of Calisthenics', 
+                'short_name' =&gt; 'Reynella-Braeview ', 
+                'contact'    =&gt; 'Tamara: 0433255991', 
+                'email'      =&gt; 'tamarabuley@hotmail.com', 
+                'location'   =&gt; 'Braeview Primary School &amp; Reynella East Primary School', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -5564,8 +5824,22 @@
       <c r="I14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 5, 
+                'full_name'  =&gt; 'Brighton Calisthenics Club', 
+                'short_name' =&gt; 'Brighton ', 
+                'contact'    =&gt; 'Catherine Tilley - 8298 1766 or 0410 581 048', 
+                'email'      =&gt; 'brightoncalisthenics@hotmail.com', 
+                'location'   =&gt; 'Brighton Uniting Church, 443 Brighton Rd', 
+                'website'    =&gt; 'www.brightoncalisthenicsclub.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37">
         <v>5</v>
       </c>
@@ -5591,8 +5865,22 @@
       <c r="I15" s="37" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 5, 
+                'full_name'  =&gt; 'Plympton Halifax', 
+                'short_name' =&gt; 'Plympton Halifax', 
+                'contact'    =&gt; 'Lisa - 0438808967', 
+                'email'      =&gt; '', 
+                'location'   =&gt; 'All Saints Uniting Church, cnr Mooringe &amp; Marion Rds, Plympton', 
+                'website'    =&gt; 'www.plymptonhalifax.org.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -5621,8 +5909,22 @@
       <c r="I16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 5, 
+                'full_name'  =&gt; 'Seacliff Calisthenics', 
+                'short_name' =&gt; 'Seacliff ', 
+                'contact'    =&gt; 'Annette Simpson: 0409 094 977', 
+                'email'      =&gt; 'seacliffcalisthenicsclub@gmail.com', 
+                'location'   =&gt; 'Seacliff Youth Centre, Yacca Rd, Seacliff', 
+                'website'    =&gt; 'www.seacliffyouthcalisthenicsclub.websyte.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -5648,8 +5950,22 @@
       <c r="I17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 6, 
+                'full_name'  =&gt; 'Largs North', 
+                'short_name' =&gt; 'Largs North', 
+                'contact'    =&gt; 'Rachel - 0431920491', 
+                'email'      =&gt; 'largsnorthcalisthenics@hotmail.com', 
+                'location'   =&gt; '', 
+                'website'    =&gt; 'www.largsnorthcalisthenics.com', 
+            ],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -5675,8 +5991,22 @@
       <c r="H18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Tonique Studio', 
+                'short_name' =&gt; 'Tonique ', 
+                'contact'    =&gt; 'Tonya: 0407809714, Monique: 0438 255 576', 
+                'email'      =&gt; 'toniquestudio@hotmail.com', 
+                'location'   =&gt; 'Glenburnie', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -5702,8 +6032,22 @@
       <c r="H19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Kangaroo Island', 
+                'short_name' =&gt; 'Kangaroo Island', 
+                'contact'    =&gt; 'Lucy: 0437995023', 
+                'email'      =&gt; 'kicalisthenics@gmail.com', 
+                'location'   =&gt; 'Parndana Town Hall', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -5732,8 +6076,22 @@
       <c r="I20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Krymzon Academy of Calisthenics', 
+                'short_name' =&gt; 'Krymzon ', 
+                'contact'    =&gt; 'Christiane : 0435 818 549', 
+                'email'      =&gt; 'christianeellis87@gmail.com', 
+                'location'   =&gt; 'Moorak', 
+                'website'    =&gt; 'www.krymzon.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -5756,8 +6114,22 @@
       <c r="H21" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Naracoorte', 
+                'short_name' =&gt; 'Naracoorte', 
+                'contact'    =&gt; 'Deb Pearce Ph. 08 8762 0296', 
+                'email'      =&gt; '', 
+                'location'   =&gt; 'Naracoorte Primary School, Park Terrace, Naracoorte', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -5783,8 +6155,22 @@
       <c r="H22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Pt Augusta', 
+                'short_name' =&gt; 'Pt Augusta', 
+                'contact'    =&gt; 'Christopher: 0417847536', 
+                'email'      =&gt; 'Secretary.portaugustacc@gmail.com', 
+                'location'   =&gt; '5 Gibson Street, Port Augusta', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7</v>
       </c>
@@ -5810,8 +6196,22 @@
       <c r="H23" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Pt Lincoln', 
+                'short_name' =&gt; 'Pt Lincoln', 
+                'contact'    =&gt; 'Renaye:0400265130', 
+                'email'      =&gt; 'portlincolncali@hotmail.com', 
+                'location'   =&gt; 'Port Lincoln', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7</v>
       </c>
@@ -5834,8 +6234,22 @@
       <c r="H24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Synergy', 
+                'short_name' =&gt; 'Synergy', 
+                'contact'    =&gt; 'Kym Lindner: 8723 3728', 
+                'email'      =&gt; '', 
+                'location'   =&gt; 'Ripley Arcade, 1st Floor, Mt Gambier', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -5858,8 +6272,22 @@
       <c r="H25" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 7, 
+                'full_name'  =&gt; 'Whydale', 
+                'short_name' =&gt; 'Whydale', 
+                'contact'    =&gt; 'Natasha Skinner: 0421 441 845', 
+                'email'      =&gt; '', 
+                'location'   =&gt; 'McRitchie Cr Hall, Whyalla', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -5888,8 +6316,22 @@
       <c r="I26" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Carisbrook', 
+                'short_name' =&gt; 'Carisbrook', 
+                'contact'    =&gt; 'Kerry : 0402 411 771', 
+                'email'      =&gt; 'carisbrookcali@gmail.com ', 
+                'location'   =&gt; 'Salisbury Uniting Church', 
+                'website'    =&gt; 'www.facebook.com/carisbrookcalisthenicsclub', 
+            ],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8</v>
       </c>
@@ -5915,8 +6357,22 @@
       <c r="H27" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Elizabeth Eastside', 
+                'short_name' =&gt; 'Elizabeth Eastside', 
+                'contact'    =&gt; 'Kate: 0412 598 195', 
+                'email'      =&gt; 'elizeastside@gmail.com', 
+                'location'   =&gt; 'Elizabeth East Primary, Dolphin St', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
@@ -5942,8 +6398,22 @@
       <c r="H28" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Gleneliz', 
+                'short_name' =&gt; 'Gleneliz', 
+                'contact'    =&gt; 'Jasmin - 0403566175', 
+                'email'      =&gt; 'gleneliz.secretary@yahoo.com.au', 
+                'location'   =&gt; 'Edinburgh North', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8</v>
       </c>
@@ -5972,8 +6442,22 @@
       <c r="I29" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Golden Heights', 
+                'short_name' =&gt; 'Golden Heights', 
+                'contact'    =&gt; 'Kerri-Anne Clarke: 0410 516 270', 
+                'email'      =&gt; 'ghcaliclub@gmail.com', 
+                'location'   =&gt; 'Golden Grove Community Centre', 
+                'website'    =&gt; 'www.goldenheightscalisthenicsclub.com', 
+            ],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>8</v>
       </c>
@@ -6002,8 +6486,22 @@
       <c r="I30" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Jem Calisthenics College', 
+                'short_name' =&gt; 'Jem ', 
+                'contact'    =&gt; 'Sonia - 0417 826 563', 
+                'email'      =&gt; 'jemcalisthenics@gmail.com', 
+                'location'   =&gt; '4&amp;5 25 Research Rd, Pooraka', 
+                'website'    =&gt; 'jemcalisthenicscollege.com', 
+            ],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>8</v>
       </c>
@@ -6029,8 +6527,22 @@
       <c r="H31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Northern Districts', 
+                'short_name' =&gt; 'Northern Districts', 
+                'contact'    =&gt; 'Lee Yon: 0411 174 741', 
+                'email'      =&gt; 'secretary@northerndistrictscalisthenicsclub.com', 
+                'location'   =&gt; 'Salisbury Park Primary, Goddard Dr. Salisbury Park &amp; St. John's Church, Church St. Salisbury', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>8</v>
       </c>
@@ -6059,8 +6571,22 @@
       <c r="I32" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Para Vista', 
+                'short_name' =&gt; 'Para Vista', 
+                'contact'    =&gt; 'Neroli : 0449 24742', 
+                'email'      =&gt; 'paravistacalisthenics@hotmail.com', 
+                'location'   =&gt; 'East Para Primary School', 
+                'website'    =&gt; 'www.paravistacalisthenics.org.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>8</v>
       </c>
@@ -6086,8 +6612,22 @@
       <c r="H33" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Payton Calisthenics College', 
+                'short_name' =&gt; 'Payton ', 
+                'contact'    =&gt; 'Dianne Ryan 0412 197 863', 
+                'email'      =&gt; 'payton.cali@gmail.com', 
+                'location'   =&gt; 'Pooraka Memorial Hall', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8</v>
       </c>
@@ -6113,8 +6653,22 @@
       <c r="H34" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 8, 
+                'full_name'  =&gt; 'Northern Vixens - Masters Only', 
+                'short_name' =&gt; 'Northern Vixens', 
+                'contact'    =&gt; 'Sharyn : 0400224055', 
+                'email'      =&gt; 'sharynrichter@bigpond.com', 
+                'location'   =&gt; 'Salisbury Downs', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>9</v>
       </c>
@@ -6143,8 +6697,22 @@
       <c r="I35" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 9, 
+                'full_name'  =&gt; 'Aurora', 
+                'short_name' =&gt; 'Aurora', 
+                'contact'    =&gt; 'Marie Pickering: 0417 827 584', 
+                'email'      =&gt; 'aurora.cali.college@gmail.com', 
+                'location'   =&gt; 'RSL Memorial Hall, Memorial Dr, Tea Tree Gully', 
+                'website'    =&gt; 'www.aurora-calisthenics.websyte.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>9</v>
       </c>
@@ -6173,8 +6741,22 @@
       <c r="I36" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 9, 
+                'full_name'  =&gt; 'Highbury', 
+                'short_name' =&gt; 'Highbury', 
+                'contact'    =&gt; 'Kathrine : 0437716808', 
+                'email'      =&gt; 'highburycali@gmail.com', 
+                'location'   =&gt; 'Hope Valley Institute, Valley Rd', 
+                'website'    =&gt; 'www.highburycalisthenics.com', 
+            ],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>9</v>
       </c>
@@ -6203,8 +6785,22 @@
       <c r="I37" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 9, 
+                'full_name'  =&gt; 'Ridgehaven', 
+                'short_name' =&gt; 'Ridgehaven', 
+                'contact'    =&gt; 'Phone  – Tracey Emes - 0412 080 854', 
+                'email'      =&gt; ' Temes8@optusnet.com.auWebsite – ', 
+                'location'   =&gt; 'Modbury Uniting Church', 
+                'website'    =&gt; 'www.ridgehavencalisthenics.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>9</v>
       </c>
@@ -6230,8 +6826,22 @@
       <c r="I38" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 9, 
+                'full_name'  =&gt; 'Windsor', 
+                'short_name' =&gt; 'Windsor', 
+                'contact'    =&gt; 'Rachel: 0401 592 919', 
+                'email'      =&gt; ' windsor.calisthenics.club@gmail.com', 
+                'location'   =&gt; '', 
+                'website'    =&gt; 'Website:  www.windsorcalisthenics.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>10</v>
       </c>
@@ -6257,8 +6867,22 @@
       <c r="I39" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 10, 
+                'full_name'  =&gt; 'Seaford', 
+                'short_name' =&gt; 'Seaford', 
+                'contact'    =&gt; 'Telisha Bayly: 0421 212 562', 
+                'email'      =&gt; 'Seafordcalisthenics@gmail.com', 
+                'location'   =&gt; '', 
+                'website'    =&gt; 'www.seafordcalisthenicsclub.org.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>10</v>
       </c>
@@ -6287,8 +6911,22 @@
       <c r="I40" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 10, 
+                'full_name'  =&gt; 'Cherum', 
+                'short_name' =&gt; 'Cherum', 
+                'contact'    =&gt; 'Sally Delaat: 0426 268 119 or Michelle Tromp: 0423 769 467', 
+                'email'      =&gt; 'cherumcali@gmail.com', 
+                'location'   =&gt; 'Christies Beach Uniting Church', 
+                'website'    =&gt; 'WWW.cherumcalisthenics.com', 
+            ],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>11</v>
       </c>
@@ -6314,8 +6952,22 @@
       <c r="H41" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 11, 
+                'full_name'  =&gt; 'Del Sante Gardens', 
+                'short_name' =&gt; 'Del Sante Gardens', 
+                'contact'    =&gt; 'Lauren Mazzachi: 0414 744 884', 
+                'email'      =&gt; 'delsantesecretary@gmail.com', 
+                'location'   =&gt; 'Flinders Park Primary School', 
+                'website'    =&gt; '', 
+            ],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>11</v>
       </c>
@@ -6344,8 +6996,22 @@
       <c r="I42" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 11, 
+                'full_name'  =&gt; 'Seaton', 
+                'short_name' =&gt; 'Seaton', 
+                'contact'    =&gt; 'Susan : 0420 989 007', 
+                'email'      =&gt; 'seatoncalisthenics@hotmail.com', 
+                'location'   =&gt; 'Seaton Baptist Church, cnr Trimmer Pde &amp; Tapleys Hill Road, Seaton', 
+                'website'    =&gt; 'www.seatoncalisthenics.com.au', 
+            ],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>11</v>
       </c>
@@ -6373,6 +7039,20 @@
       </c>
       <c r="I43" t="s">
         <v>155</v>
+      </c>
+      <c r="J43" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                'region_id'  =&gt; 11, 
+                'full_name'  =&gt; 'Seaview Calisthenics College', 
+                'short_name' =&gt; 'Seaview ', 
+                'contact'    =&gt; 'Renee 0439 186 734', 
+                'email'      =&gt; 'seaviewcalisthenicscollege@gmail.com', 
+                'location'   =&gt; 'Henley Town Hall, Henley Beach', 
+                'website'    =&gt; 'www.seaviewcalisthenics.org', 
+            ],</v>
       </c>
     </row>
   </sheetData>
@@ -6394,20 +7074,21 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC4D618-95C1-8348-BD50-5B638D546115}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -6415,106 +7096,151 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="str">
+        <f>"            [ 'id' =&gt; "&amp;A2&amp;", 'name' =&gt; '"&amp;B2&amp;"' ],"</f>
+        <v xml:space="preserve">            [ 'id' =&gt; 1, 'name' =&gt; 'Adelaide Hills' ],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C12" si="0">"            [ 'id' =&gt; "&amp;A3&amp;", 'name' =&gt; '"&amp;B3&amp;"' ],"</f>
+        <v xml:space="preserve">            [ 'id' =&gt; 2, 'name' =&gt; 'Country North' ],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 3, 'name' =&gt; 'Metropolitan East' ],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 4, 'name' =&gt; 'Metropolitan South' ],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 5, 'name' =&gt; 'Metropolitan South West' ],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 6, 'name' =&gt; 'Metropolitan North West' ],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 7, 'name' =&gt; 'Regional' ],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 8, 'name' =&gt; 'Metropolitan North' ],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 9, 'name' =&gt; 'Metropolitan North East' ],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 10, 'name' =&gt; 'Metropolitan Outer South' ],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>144</v>
       </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'id' =&gt; 11, 'name' =&gt; 'Metropolitan West' ],</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C12" xr:uid="{9DA7841A-5CCD-BF43-BC50-4014605D1CAB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C3E24B-EBEA-3C43-9A9A-131872B7DFCF}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6522,9 +7248,10 @@
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>172</v>
       </c>
@@ -6544,12 +7271,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>1174</v>
       </c>
       <c r="C2" s="3">
         <v>6.25E-2</v>
@@ -6563,13 +7290,17 @@
       <c r="F2" s="3">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I2" t="str">
+        <f>"            [ 'sequence' =&gt; "&amp;A2&amp;", 'name' =&gt; '"&amp;B2&amp;"' ],"</f>
+        <v xml:space="preserve">            [ 'sequence' =&gt; 110, 'name' =&gt; 'Non Competitive Tinies ' ],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" s="3">
         <v>6.25E-2</v>
@@ -6583,39 +7314,47 @@
       <c r="F3" s="3">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I8" si="0">"            [ 'sequence' =&gt; "&amp;A3&amp;", 'name' =&gt; '"&amp;B3&amp;"' ],"</f>
+        <v xml:space="preserve">            [ 'sequence' =&gt; 120, 'name' =&gt; 'Competitive Tinies ' ],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'sequence' =&gt; 130, 'name' =&gt; 'Sub Juniors ' ],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
         <v>1105</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="3">
         <v>0.125</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.14583333333333334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1103</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.14583333333333334</v>
       </c>
       <c r="E5" s="3">
         <v>0.10416666666666667</v>
@@ -6623,13 +7362,17 @@
       <c r="F5" s="3">
         <v>0.14583333333333334</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'sequence' =&gt; 140, 'name' =&gt; 'Juniors' ],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C6" s="3">
         <v>0.10416666666666667</v>
@@ -6643,13 +7386,17 @@
       <c r="F6" s="3">
         <v>0.14583333333333334</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'sequence' =&gt; 150, 'name' =&gt; 'Intermediates' ],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>1104</v>
       </c>
       <c r="C7" s="3">
         <v>0.10416666666666667</v>
@@ -6658,10 +7405,38 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="E7" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'sequence' =&gt; 160, 'name' =&gt; 'Seniors' ],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>170</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E8" s="3">
         <v>0.125</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="3">
         <v>0.16666666666666666</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            [ 'sequence' =&gt; 170, 'name' =&gt; 'Masters' ],</v>
       </c>
     </row>
   </sheetData>
@@ -32802,7 +33577,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD53"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47060,323 +47835,323 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="60" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
+      <c r="A7" s="58" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="52" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G8" s="55"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="52" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F9" s="55"/>
+      <c r="G9" s="53" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="52" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="52" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F11" s="50" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="52" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>940</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="59" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="61"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+    </row>
+    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.2">
+      <c r="A16" s="58" t="s">
         <v>1167</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+    </row>
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="52" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C17" s="56"/>
+      <c r="D17" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G17" s="55"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="52" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G18" s="50" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="52" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G19" s="50" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="52" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F20" s="50" t="s">
+        <v>940</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="52" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G21" s="50" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
         <v>1163</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="54" t="s">
+      <c r="B22" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C22" s="51" t="s">
         <v>1161</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="D22" s="51" t="s">
         <v>1160</v>
       </c>
-      <c r="F8" s="53" t="s">
-        <v>1169</v>
-      </c>
-      <c r="G8" s="58"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="55" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B9" s="57" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="56" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="55" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B10" s="54" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E10" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F10" s="53" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="55" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B11" s="54" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55" t="s">
-        <v>1104</v>
-      </c>
-      <c r="B12" s="57" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C12" s="57" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D12" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E12" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>940</v>
-      </c>
-      <c r="G12" s="53" t="s">
+      <c r="E22" s="51" t="s">
         <v>1159</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B13" s="54" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D13" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F13" s="53" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G13" s="53" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
+      <c r="F22" s="50" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G22" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="50"/>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="61"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-    </row>
-    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.2">
-      <c r="A16" s="60" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B17" s="54" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E17" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F17" s="53" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G17" s="58"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="55" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B18" s="54" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E18" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F18" s="56" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G18" s="53" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B19" s="57" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C19" s="54" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D19" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E19" s="57" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G19" s="53" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="55" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B20" s="57" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D20" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E20" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F20" s="53" t="s">
-        <v>940</v>
-      </c>
-      <c r="G20" s="56" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="55" t="s">
-        <v>1104</v>
-      </c>
-      <c r="B21" s="54" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E21" s="57" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F21" s="56" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G21" s="53" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B22" s="54" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C22" s="54" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D22" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E22" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F22" s="53" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G22" s="53" t="s">
-        <v>1159</v>
-      </c>
     </row>
     <row r="23" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="50"/>
+      <c r="A23" s="59" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -47395,9 +48170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1DE507D-BFDC-1044-ACF7-E9B623FDD1E5}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47412,10 +48187,10 @@
         <v>1126</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -47426,7 +48201,7 @@
         <v>934</v>
       </c>
       <c r="C2" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -47434,10 +48209,10 @@
         <v>1124</v>
       </c>
       <c r="B3" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -47448,7 +48223,7 @@
         <v>941</v>
       </c>
       <c r="C4" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -47459,7 +48234,7 @@
         <v>929</v>
       </c>
       <c r="C5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -47467,10 +48242,10 @@
         <v>1123</v>
       </c>
       <c r="B7" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C7" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -47511,10 +48286,10 @@
         <v>1123</v>
       </c>
       <c r="B11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -47522,10 +48297,10 @@
         <v>1123</v>
       </c>
       <c r="B12" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C12" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -47533,10 +48308,10 @@
         <v>1123</v>
       </c>
       <c r="B13" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C13" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -47544,10 +48319,10 @@
         <v>1123</v>
       </c>
       <c r="B14" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C14" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -47566,43 +48341,43 @@
         <v>1123</v>
       </c>
       <c r="B16" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C16" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B18" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C18" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B19" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C19" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B20" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C20" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "has music title" as a field on the item type
</commit_message>
<xml_diff>
--- a/doco/caliad.xlsx
+++ b/doco/caliad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendantwhite/code/caliad/doco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8541BE1F-0291-D445-BE9E-6FB9E3C31B56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E7424B-9986-4942-9C0C-03225A914EA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
   </bookViews>
@@ -3945,12 +3945,6 @@
     <t>CommYear</t>
   </si>
   <si>
-    <t>HasMusic?</t>
-  </si>
-  <si>
-    <t>EveryYear?</t>
-  </si>
-  <si>
     <t>Seq</t>
   </si>
   <si>
@@ -4087,6 +4081,12 @@
   </si>
   <si>
     <t>Laravel</t>
+  </si>
+  <si>
+    <t>Music Title</t>
+  </si>
+  <si>
+    <t>HasMusicTitle</t>
   </si>
 </sst>
 </file>
@@ -4461,6 +4461,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4473,10 +4477,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4849,33 +4849,33 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="13.83203125" style="64"/>
-    <col min="9" max="10" width="13.83203125" style="64"/>
+    <col min="1" max="6" width="13.83203125" style="60"/>
+    <col min="9" max="10" width="13.83203125" style="60"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="58" t="s">
         <v>1121</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="58" t="s">
         <v>944</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="58" t="s">
         <v>1087</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="58" t="s">
         <v>1133</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="58" t="s">
         <v>1127</v>
       </c>
       <c r="G1" s="39" t="s">
@@ -4884,10 +4884,10 @@
       <c r="H1" s="39" t="s">
         <v>1108</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="58" t="s">
         <v>1126</v>
       </c>
       <c r="K1" s="39" t="s">
@@ -4900,27 +4900,27 @@
         <v>1129</v>
       </c>
       <c r="N1" s="39" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="59" t="s">
         <v>1133</v>
       </c>
       <c r="H2" s="45" t="s">
         <v>1127</v>
       </c>
-      <c r="I2" s="63" t="s">
+      <c r="I2" s="59" t="s">
         <v>1126</v>
       </c>
-      <c r="J2" s="63"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="45" t="s">
         <v>1087</v>
       </c>
@@ -4935,17 +4935,17 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
       <c r="H3" s="45" t="s">
         <v>1121</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
       <c r="K3" s="45" t="s">
         <v>1121</v>
       </c>
@@ -4960,54 +4960,54 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="63"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
       <c r="H4" s="45" t="s">
         <v>1130</v>
       </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
       <c r="K4" s="45" t="s">
         <v>1131</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="63"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
       <c r="H5" s="45" t="s">
         <v>1132</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
       <c r="K5" s="45" t="s">
         <v>1133</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="64" t="s">
-        <v>1145</v>
-      </c>
-      <c r="E7" s="64" t="s">
+      <c r="D7" s="60" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E7" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="60" t="s">
         <v>157</v>
       </c>
       <c r="G7" t="s">
@@ -5016,79 +5016,80 @@
       <c r="H7" s="46" t="s">
         <v>1135</v>
       </c>
-      <c r="I7" s="65" t="s">
-        <v>1145</v>
-      </c>
-      <c r="J7" s="65" t="s">
+      <c r="I7" s="61" t="s">
+        <v>1143</v>
+      </c>
+      <c r="J7" s="61" t="s">
         <v>157</v>
       </c>
       <c r="L7" t="s">
+        <v>1138</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1138</v>
+      </c>
+      <c r="N7" t="s">
         <v>1140</v>
       </c>
-      <c r="M7" t="s">
-        <v>1140</v>
-      </c>
-      <c r="N7" t="s">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="60" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D8" s="60" t="s">
         <v>1142</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="64" t="s">
-        <v>1136</v>
-      </c>
-      <c r="B8" s="64" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E8" s="64" t="s">
+      <c r="E8" s="60" t="s">
         <v>1137</v>
       </c>
-      <c r="F8" s="64" t="s">
-        <v>1175</v>
-      </c>
-      <c r="I8" s="64" t="s">
-        <v>1144</v>
-      </c>
-      <c r="J8" s="64" t="s">
-        <v>1139</v>
+      <c r="F8" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I8" s="60" t="s">
+        <v>1142</v>
+      </c>
+      <c r="J8" s="60" t="s">
+        <v>1178</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1177</v>
       </c>
       <c r="N8" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="64" t="s">
-        <v>1176</v>
-      </c>
-      <c r="I9" s="64" t="s">
-        <v>1173</v>
-      </c>
-      <c r="J9" s="65" t="s">
-        <v>1138</v>
-      </c>
+      <c r="F9" s="60" t="s">
+        <v>1174</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J9" s="61"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="60" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="60" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="60" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="60" t="s">
         <v>162</v>
       </c>
     </row>
@@ -5265,10 +5266,10 @@
         <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>161</v>
@@ -5283,10 +5284,10 @@
         <v>162</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -5316,7 +5317,7 @@
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K2" t="str">
         <f>_xlfn.CONCAT("                'region_id'  =&gt; "&amp;A2&amp;", 
@@ -5364,7 +5365,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K43" si="0">_xlfn.CONCAT("                'region_id'  =&gt; "&amp;A3&amp;", 
@@ -5412,7 +5413,7 @@
         <v>180</v>
       </c>
       <c r="J4" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
@@ -5453,7 +5454,7 @@
         <v>9</v>
       </c>
       <c r="J5" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
@@ -5491,7 +5492,7 @@
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -5529,7 +5530,7 @@
         <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -5570,7 +5571,7 @@
         <v>22</v>
       </c>
       <c r="J8" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -5614,7 +5615,7 @@
         <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -5655,7 +5656,7 @@
         <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -5696,7 +5697,7 @@
         <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
@@ -5740,7 +5741,7 @@
         <v>179</v>
       </c>
       <c r="J12" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -5781,7 +5782,7 @@
         <v>40</v>
       </c>
       <c r="J13" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
@@ -5825,7 +5826,7 @@
         <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
@@ -5866,7 +5867,7 @@
         <v>51</v>
       </c>
       <c r="J15" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
@@ -5910,7 +5911,7 @@
         <v>56</v>
       </c>
       <c r="J16" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
@@ -5951,7 +5952,7 @@
         <v>61</v>
       </c>
       <c r="J17" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
@@ -5992,7 +5993,7 @@
         <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
@@ -6033,7 +6034,7 @@
         <v>67</v>
       </c>
       <c r="J19" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
@@ -6077,7 +6078,7 @@
         <v>73</v>
       </c>
       <c r="J20" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
@@ -6115,7 +6116,7 @@
         <v>76</v>
       </c>
       <c r="J21" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
@@ -6156,7 +6157,7 @@
         <v>79</v>
       </c>
       <c r="J22" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="0"/>
@@ -6197,7 +6198,7 @@
         <v>83</v>
       </c>
       <c r="J23" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
@@ -6235,7 +6236,7 @@
         <v>87</v>
       </c>
       <c r="J24" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
@@ -6273,7 +6274,7 @@
         <v>90</v>
       </c>
       <c r="J25" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="0"/>
@@ -6317,7 +6318,7 @@
         <v>95</v>
       </c>
       <c r="J26" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="0"/>
@@ -6358,7 +6359,7 @@
         <v>97</v>
       </c>
       <c r="J27" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="0"/>
@@ -6399,7 +6400,7 @@
         <v>99</v>
       </c>
       <c r="J28" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="0"/>
@@ -6443,7 +6444,7 @@
         <v>106</v>
       </c>
       <c r="J29" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="0"/>
@@ -6487,7 +6488,7 @@
         <v>178</v>
       </c>
       <c r="J30" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
@@ -6528,7 +6529,7 @@
         <v>111</v>
       </c>
       <c r="J31" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="0"/>
@@ -6572,7 +6573,7 @@
         <v>116</v>
       </c>
       <c r="J32" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="0"/>
@@ -6613,7 +6614,7 @@
         <v>118</v>
       </c>
       <c r="J33" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="0"/>
@@ -6654,7 +6655,7 @@
         <v>120</v>
       </c>
       <c r="J34" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="0"/>
@@ -6698,7 +6699,7 @@
         <v>182</v>
       </c>
       <c r="J35" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="0"/>
@@ -6742,7 +6743,7 @@
         <v>130</v>
       </c>
       <c r="J36" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="0"/>
@@ -6786,7 +6787,7 @@
         <v>133</v>
       </c>
       <c r="J37" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="0"/>
@@ -6827,7 +6828,7 @@
         <v>135</v>
       </c>
       <c r="J38" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="0"/>
@@ -6868,7 +6869,7 @@
         <v>181</v>
       </c>
       <c r="J39" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="0"/>
@@ -6912,7 +6913,7 @@
         <v>143</v>
       </c>
       <c r="J40" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="0"/>
@@ -6953,7 +6954,7 @@
         <v>146</v>
       </c>
       <c r="J41" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="0"/>
@@ -6997,7 +6998,7 @@
         <v>151</v>
       </c>
       <c r="J42" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="0"/>
@@ -7041,7 +7042,7 @@
         <v>155</v>
       </c>
       <c r="J43" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K43" t="str">
         <f t="shared" si="0"/>
@@ -7276,7 +7277,7 @@
         <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="C2" s="3">
         <v>6.25E-2</v>
@@ -47835,50 +47836,50 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
+      <c r="A7" s="62" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F8" s="50" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E9" s="54" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F9" s="55"/>
       <c r="G9" s="53" t="s">
@@ -47890,19 +47891,19 @@
         <v>1105</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="G10" s="53" t="s">
         <v>933</v>
@@ -47913,19 +47914,19 @@
         <v>1103</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F11" s="50" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="G11" s="53" t="s">
         <v>939</v>
@@ -47936,57 +47937,57 @@
         <v>1104</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E12" s="51" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F12" s="53" t="s">
         <v>940</v>
       </c>
       <c r="G12" s="50" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F13" s="50" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="G13" s="50" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
-        <v>1157</v>
-      </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="61"/>
+      <c r="A14" s="63" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="57"/>
@@ -47998,56 +47999,56 @@
       <c r="G15" s="57"/>
     </row>
     <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.2">
-      <c r="A16" s="58" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
+      <c r="A16" s="62" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F17" s="50" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="B18" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G18" s="50" t="s">
         <v>1162</v>
-      </c>
-      <c r="C18" s="54" t="s">
-        <v>1161</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>1160</v>
-      </c>
-      <c r="E18" s="51" t="s">
-        <v>1159</v>
-      </c>
-      <c r="F18" s="53" t="s">
-        <v>1147</v>
-      </c>
-      <c r="G18" s="50" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -48055,19 +48056,19 @@
         <v>1105</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="G19" s="50" t="s">
         <v>942</v>
@@ -48078,22 +48079,22 @@
         <v>1103</v>
       </c>
       <c r="B20" s="54" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F20" s="50" t="s">
         <v>940</v>
       </c>
       <c r="G20" s="53" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -48101,19 +48102,19 @@
         <v>1104</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E21" s="54" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F21" s="53" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="G21" s="50" t="s">
         <v>933</v>
@@ -48121,37 +48122,37 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F22" s="50" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="G22" s="50" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="59" t="s">
-        <v>1157</v>
-      </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61"/>
+      <c r="A23" s="63" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -48187,10 +48188,10 @@
         <v>1126</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -48201,7 +48202,7 @@
         <v>934</v>
       </c>
       <c r="C2" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -48209,10 +48210,10 @@
         <v>1124</v>
       </c>
       <c r="B3" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C3" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -48223,7 +48224,7 @@
         <v>941</v>
       </c>
       <c r="C4" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -48234,7 +48235,7 @@
         <v>929</v>
       </c>
       <c r="C5" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -48242,10 +48243,10 @@
         <v>1123</v>
       </c>
       <c r="B7" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="C7" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -48286,10 +48287,10 @@
         <v>1123</v>
       </c>
       <c r="B11" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C11" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -48297,10 +48298,10 @@
         <v>1123</v>
       </c>
       <c r="B12" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C12" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -48308,10 +48309,10 @@
         <v>1123</v>
       </c>
       <c r="B13" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="C13" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -48319,10 +48320,10 @@
         <v>1123</v>
       </c>
       <c r="B14" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="C14" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -48341,43 +48342,43 @@
         <v>1123</v>
       </c>
       <c r="B16" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C16" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="B18" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C18" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="B19" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="C19" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="B20" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C20" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
team rank database and data
</commit_message>
<xml_diff>
--- a/doco/caliad.xlsx
+++ b/doco/caliad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendantwhite/code/caliad/doco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E7424B-9986-4942-9C0C-03225A914EA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D016172-E7DF-FF4B-A26D-FD67F657844B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
   </bookViews>
@@ -4849,12 +4849,12 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="13.83203125" style="60"/>
+    <col min="1" max="7" width="13.83203125" style="60"/>
     <col min="9" max="10" width="13.83203125" style="60"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -4878,7 +4878,7 @@
       <c r="F1" s="58" t="s">
         <v>1127</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="58" t="s">
         <v>1131</v>
       </c>
       <c r="H1" s="39" t="s">
@@ -4914,6 +4914,7 @@
       <c r="F2" s="59" t="s">
         <v>1133</v>
       </c>
+      <c r="G2" s="59"/>
       <c r="H2" s="45" t="s">
         <v>1127</v>
       </c>
@@ -4941,6 +4942,7 @@
       <c r="D3" s="59"/>
       <c r="E3" s="59"/>
       <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
       <c r="H3" s="45" t="s">
         <v>1121</v>
       </c>
@@ -4966,6 +4968,7 @@
       <c r="D4" s="59"/>
       <c r="E4" s="59"/>
       <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="45" t="s">
         <v>1130</v>
       </c>
@@ -4982,6 +4985,7 @@
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
       <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="45" t="s">
         <v>1132</v>
       </c>
@@ -5010,7 +5014,7 @@
       <c r="F7" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="60" t="s">
         <v>1136</v>
       </c>
       <c r="H7" s="46" t="s">
@@ -33578,7 +33582,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+      <selection pane="bottomLeft" activeCell="F333" sqref="F333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
db changes for Routines
</commit_message>
<xml_diff>
--- a/doco/caliad.xlsx
+++ b/doco/caliad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendantwhite/code/caliad/doco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E385B08-8642-6048-9B1E-E32A3CFEC0A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9F5391-F75D-924F-ACAF-3DB93CE99146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9639" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9641" uniqueCount="1184">
   <si>
     <t>Adelaide Hills</t>
   </si>
@@ -4096,6 +4096,12 @@
   </si>
   <si>
     <t>Cohort</t>
+  </si>
+  <si>
+    <t>StartTimeDate</t>
+  </si>
+  <si>
+    <t>EndTimeDate</t>
   </si>
 </sst>
 </file>
@@ -4362,7 +4368,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4475,7 +4481,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4523,14 +4528,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4903,59 +4904,56 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="13.83203125" style="60"/>
-    <col min="8" max="8" width="13.83203125" style="30"/>
-    <col min="9" max="9" width="13.83203125" style="69"/>
-    <col min="10" max="11" width="13.83203125" style="60"/>
+    <col min="1" max="14" width="13.83203125" style="59"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="39" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>1121</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="57" t="s">
         <v>944</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>1087</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="57" t="s">
         <v>1133</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="57" t="s">
         <v>1127</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>1131</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="65" t="s">
         <v>1181</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="57" t="s">
         <v>950</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="57" t="s">
         <v>1126</v>
       </c>
-      <c r="K1" s="58" t="s">
+      <c r="K1" s="57" t="s">
         <v>253</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="57" t="s">
         <v>1108</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="57" t="s">
         <v>1134</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="57" t="s">
         <v>1129</v>
       </c>
       <c r="O1" s="39" t="s">
@@ -4963,34 +4961,34 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59" t="s">
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="58" t="s">
         <v>1133</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="71" t="s">
+      <c r="G2" s="58"/>
+      <c r="H2" s="66" t="s">
         <v>1087</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="58" t="s">
         <v>1179</v>
       </c>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>1126</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="58" t="s">
         <v>1127</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="58" t="s">
         <v>1108</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="58" t="s">
         <v>950</v>
       </c>
       <c r="O2" s="45" t="s">
@@ -4998,28 +4996,28 @@
       </c>
     </row>
     <row r="3" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="72" t="s">
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="67" t="s">
         <v>1180</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="58" t="s">
         <v>1131</v>
       </c>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="45" t="s">
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58" t="s">
         <v>1121</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="N3" s="45" t="s">
+      <c r="N3" s="58" t="s">
         <v>1128</v>
       </c>
       <c r="O3" s="45" t="s">
@@ -5027,76 +5025,80 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="45" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="73" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="68" t="s">
         <v>1133</v>
       </c>
-      <c r="I4" s="68"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="45" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58" t="s">
         <v>1130</v>
       </c>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
     </row>
     <row r="5" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="66" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58" t="s">
         <v>944</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="45" t="s">
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58" t="s">
         <v>1132</v>
       </c>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="59" t="s">
         <v>1143</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="59" t="s">
         <v>1136</v>
       </c>
-      <c r="J7" s="61" t="s">
+      <c r="J7" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="K7" s="61" t="s">
+      <c r="K7" s="60" t="s">
         <v>1143</v>
       </c>
-      <c r="L7" s="46" t="s">
+      <c r="L7" s="60" t="s">
         <v>1135</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="59" t="s">
         <v>1138</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="59" t="s">
         <v>1138</v>
       </c>
       <c r="O7" t="s">
@@ -5104,28 +5106,28 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="59" t="s">
         <v>1136</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="59" t="s">
         <v>1136</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="59" t="s">
         <v>1142</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="59" t="s">
         <v>1137</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="59" t="s">
         <v>1173</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="59" t="s">
         <v>1178</v>
       </c>
-      <c r="K8" s="60" t="s">
+      <c r="K8" s="59" t="s">
         <v>1142</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="59" t="s">
         <v>1177</v>
       </c>
       <c r="O8" t="s">
@@ -5133,34 +5135,40 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="59" t="s">
         <v>1174</v>
       </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="60" t="s">
+      <c r="J9" s="60"/>
+      <c r="K9" s="59" t="s">
         <v>1171</v>
       </c>
+      <c r="N9" s="59" t="s">
+        <v>1182</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="59" t="s">
         <v>161</v>
       </c>
+      <c r="N10" s="59" t="s">
+        <v>1183</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="59" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="59" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="59" t="s">
         <v>162</v>
       </c>
     </row>
@@ -47900,330 +47908,330 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="49" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="48" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="48" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="47"/>
+    <col min="1" max="1" width="13.6640625" style="48" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="47" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="47" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="46"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>1167</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="51" t="s">
         <v>1164</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="51" t="s">
+      <c r="C8" s="55"/>
+      <c r="D8" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="49" t="s">
         <v>1166</v>
       </c>
-      <c r="G8" s="55"/>
+      <c r="G8" s="54"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="51" t="s">
         <v>1163</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="53" t="s">
         <v>1160</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="50" t="s">
         <v>1159</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="53" t="s">
         <v>1157</v>
       </c>
-      <c r="F9" s="55"/>
-      <c r="G9" s="53" t="s">
+      <c r="F9" s="54"/>
+      <c r="G9" s="52" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="51" t="s">
         <v>1105</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="53" t="s">
         <v>1159</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="53" t="s">
         <v>1158</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="49" t="s">
         <v>1145</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="52" t="s">
         <v>933</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="51" t="s">
         <v>1103</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="50" t="s">
         <v>1159</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="53" t="s">
         <v>1158</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="53" t="s">
         <v>1157</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="49" t="s">
         <v>1145</v>
       </c>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="52" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="51" t="s">
         <v>1104</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="53" t="s">
         <v>1160</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="53" t="s">
         <v>1159</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="52" t="s">
         <v>940</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="49" t="s">
         <v>1156</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="51" t="s">
         <v>1161</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="50" t="s">
         <v>1159</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="49" t="s">
         <v>1145</v>
       </c>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="49" t="s">
         <v>1156</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="62" t="s">
         <v>1155</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="65"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="64"/>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.2">
-      <c r="A16" s="62" t="s">
+      <c r="A16" s="61" t="s">
         <v>1165</v>
       </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="51" t="s">
         <v>1164</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="51" t="s">
+      <c r="C17" s="55"/>
+      <c r="D17" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F17" s="50" t="s">
+      <c r="F17" s="49" t="s">
         <v>1145</v>
       </c>
-      <c r="G17" s="55"/>
+      <c r="G17" s="54"/>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="51" t="s">
         <v>1163</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="53" t="s">
         <v>1159</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="53" t="s">
         <v>1158</v>
       </c>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="52" t="s">
         <v>1145</v>
       </c>
-      <c r="G18" s="50" t="s">
+      <c r="G18" s="49" t="s">
         <v>1162</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="51" t="s">
         <v>1105</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="53" t="s">
         <v>1160</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="50" t="s">
         <v>1159</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="53" t="s">
         <v>1157</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="52" t="s">
         <v>1145</v>
       </c>
-      <c r="G19" s="50" t="s">
+      <c r="G19" s="49" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="51" t="s">
         <v>1103</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="53" t="s">
         <v>1160</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="53" t="s">
         <v>1159</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E20" s="51" t="s">
+      <c r="E20" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="49" t="s">
         <v>940</v>
       </c>
-      <c r="G20" s="53" t="s">
+      <c r="G20" s="52" t="s">
         <v>1156</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="51" t="s">
         <v>1104</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="50" t="s">
         <v>1159</v>
       </c>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="53" t="s">
         <v>1158</v>
       </c>
-      <c r="E21" s="54" t="s">
+      <c r="E21" s="53" t="s">
         <v>1157</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="52" t="s">
         <v>1145</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="G21" s="49" t="s">
         <v>933</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="51" t="s">
         <v>1161</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="50" t="s">
         <v>1159</v>
       </c>
-      <c r="D22" s="51" t="s">
+      <c r="D22" s="50" t="s">
         <v>1158</v>
       </c>
-      <c r="E22" s="51" t="s">
+      <c r="E22" s="50" t="s">
         <v>1157</v>
       </c>
-      <c r="F22" s="50" t="s">
+      <c r="F22" s="49" t="s">
         <v>1145</v>
       </c>
-      <c r="G22" s="50" t="s">
+      <c r="G22" s="49" t="s">
         <v>1156</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="62" t="s">
         <v>1155</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="65"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
age_group_item_types database structure and data
</commit_message>
<xml_diff>
--- a/doco/caliad.xlsx
+++ b/doco/caliad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendantwhite/code/caliad/doco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9F5391-F75D-924F-ACAF-3DB93CE99146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DC8E23-1FD9-7F47-A3E1-74A549F42599}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
+    <workbookView xWindow="2480" yWindow="6840" windowWidth="28800" windowHeight="16380" activeTab="12" xr2:uid="{68D2FF76-B0A3-2841-B418-5D81E6E261B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="12" r:id="rId1"/>
@@ -4516,6 +4516,10 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4528,10 +4532,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4903,14 +4903,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD349239-A764-1A46-BD88-AF5CB97580BD}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="14" width="13.83203125" style="59"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="39" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4935,7 +4935,7 @@
       <c r="G1" s="57" t="s">
         <v>1131</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="61" t="s">
         <v>1181</v>
       </c>
       <c r="I1" s="57" t="s">
@@ -4956,7 +4956,7 @@
       <c r="N1" s="57" t="s">
         <v>1129</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="57" t="s">
         <v>1139</v>
       </c>
     </row>
@@ -4972,7 +4972,7 @@
         <v>1133</v>
       </c>
       <c r="G2" s="58"/>
-      <c r="H2" s="66" t="s">
+      <c r="H2" s="62" t="s">
         <v>1087</v>
       </c>
       <c r="I2" s="58" t="s">
@@ -4991,7 +4991,7 @@
       <c r="N2" s="58" t="s">
         <v>950</v>
       </c>
-      <c r="O2" s="45" t="s">
+      <c r="O2" s="58" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -5003,7 +5003,7 @@
       <c r="E3" s="58"/>
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="63" t="s">
         <v>1180</v>
       </c>
       <c r="I3" s="58" t="s">
@@ -5020,7 +5020,7 @@
       <c r="N3" s="58" t="s">
         <v>1128</v>
       </c>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="58" t="s">
         <v>1126</v>
       </c>
     </row>
@@ -5032,7 +5032,7 @@
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
       <c r="G4" s="58"/>
-      <c r="H4" s="68" t="s">
+      <c r="H4" s="64" t="s">
         <v>1133</v>
       </c>
       <c r="I4" s="58"/>
@@ -5043,6 +5043,7 @@
       </c>
       <c r="M4" s="58"/>
       <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
     </row>
     <row r="5" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="58"/>
@@ -5063,6 +5064,7 @@
       </c>
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -5101,7 +5103,7 @@
       <c r="N7" s="59" t="s">
         <v>1138</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="59" t="s">
         <v>1140</v>
       </c>
     </row>
@@ -5130,7 +5132,7 @@
       <c r="N8" s="59" t="s">
         <v>1177</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="59" t="s">
         <v>1141</v>
       </c>
     </row>
@@ -7318,9 +7320,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C3E24B-EBEA-3C43-9A9A-131872B7DFCF}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I8"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47915,15 +47917,15 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="65" t="s">
         <v>1167</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="51" t="s">
@@ -48058,15 +48060,15 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="66" t="s">
         <v>1155</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="68"/>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="56"/>
@@ -48078,15 +48080,15 @@
       <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="65" t="s">
         <v>1165</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
@@ -48223,15 +48225,15 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="66" t="s">
         <v>1155</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="64"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>